<commit_message>
Add Client/Server Export Setting
Now, you can use "(C)" to tag this column that can only be exported to
client file."(S)" to server file.
</commit_message>
<xml_diff>
--- a/sTools/excelTable/mapinfo.xlsx
+++ b/sTools/excelTable/mapinfo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -21,7 +21,7 @@
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0">
+    <comment ref="E2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>地图ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -91,30 +91,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>mapName(S)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>scene/TestScene</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>地图名称(客户端)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>resPath(S)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>地图信息（服务器）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>spaces/testscene</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>type(I)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -132,6 +116,33 @@
   </si>
   <si>
     <t>0,0,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>navMesh文件（客户端）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scene/newplayerscene1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>newPlayerScene1</t>
+  </si>
+  <si>
+    <t>spaces/newplayerscene1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(C)navMesh(S)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(S)resPath(S)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(C)mapName(S)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -496,68 +507,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
+      <c r="F3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change monster to entity
</commit_message>
<xml_diff>
--- a/sTools/excelTable/mapinfo.xlsx
+++ b/sTools/excelTable/mapinfo.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>地图ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -147,23 +147,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>(S)MonsterFile(S)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(S)NPCFile(S)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>npc配表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>怪物配表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>scripts\data\spawnpoints\monster_newplayermapinfo.xml</t>
+    <t>(S)EntityFile(S)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>非玩家配表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scripts\data\spawnpoints\entity_newplayermapinfo.xml</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -528,7 +520,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
@@ -541,10 +533,9 @@
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="59.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -566,11 +557,8 @@
       <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -590,13 +578,10 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>1</v>
       </c>
@@ -616,7 +601,7 @@
         <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>